<commit_message>
working on the import
</commit_message>
<xml_diff>
--- a/public/dashboard/inventorySample.xlsx
+++ b/public/dashboard/inventorySample.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">SN</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t xml:space="preserve">2B-Type5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fdfdsf</t>
   </si>
 </sst>
 </file>
@@ -61,6 +64,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -82,6 +86,7 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -156,13 +161,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.8"/>
@@ -217,6 +222,11 @@
       </c>
       <c r="G2" s="0" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>